<commit_message>
Added the MST component
</commit_message>
<xml_diff>
--- a/GuessSounds_conditions.xlsx
+++ b/GuessSounds_conditions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangs\OneDrive - The University of Western Ontario\Desktop\Project BL\Guess The Sound\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/swan689_uwo_ca/Documents/Desktop/Project BL/Guess The Sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3907C1-A3B2-41A5-B942-A30021B704D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{EF3907C1-A3B2-41A5-B942-A30021B704D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E48C104-6B01-490E-80FB-E6FB2AB7E575}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{BE90900A-ACE8-4230-85D6-181754847329}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="138">
   <si>
     <t>Type</t>
   </si>
@@ -463,7 +463,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,6 +473,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,12 +501,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294CB12A-D23A-4261-8EC5-DD7E3139FA57}">
-  <dimension ref="A1:A81"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -826,123 +840,123 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>53</v>
+      <c r="A3" s="6" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
+      <c r="A4" s="6" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>95</v>
+      <c r="A5" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>100</v>
+      <c r="A6" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>31</v>
+      <c r="A7" s="6" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>66</v>
+      <c r="A8" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>83</v>
+      <c r="A9" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>77</v>
+      <c r="A10" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
-        <v>13</v>
+      <c r="A14" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>22</v>
+      <c r="A15" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>32</v>
+      <c r="A16" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>3</v>
+      <c r="A19" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>78</v>
+      <c r="A21" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>94</v>
+      <c r="A22" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>96</v>
+      <c r="A23" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>72</v>
+      <c r="A24" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>104</v>
+      <c r="A25" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
@@ -996,7 +1010,7 @@
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1012,67 +1026,67 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
@@ -1223,6 +1237,106 @@
     <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Guess the Sound --> Sound memory task
</commit_message>
<xml_diff>
--- a/GuessSounds_conditions.xlsx
+++ b/GuessSounds_conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/swan689_uwo_ca/Documents/Desktop/Project BL/Guess The Sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{EF3907C1-A3B2-41A5-B942-A30021B704D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BCAF404A-BEEC-49FB-AC05-E18E28465399}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{4AF6C817-0FAB-4552-9560-1836CE493123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{41100F38-E1FD-4556-AE57-21E9DA2CFA91}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{BE90900A-ACE8-4230-85D6-181754847329}"/>
+    <workbookView xWindow="10450" yWindow="1020" windowWidth="12110" windowHeight="12810" xr2:uid="{BE90900A-ACE8-4230-85D6-181754847329}"/>
   </bookViews>
   <sheets>
     <sheet name="V4" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="165">
   <si>
     <t>Type</t>
   </si>
@@ -483,22 +483,46 @@
     <t>10 repeat I</t>
   </si>
   <si>
-    <t>10 repeat II</t>
-  </si>
-  <si>
     <t>10 new I</t>
   </si>
   <si>
     <t>10 new II</t>
   </si>
   <si>
-    <t>30 new</t>
-  </si>
-  <si>
     <t>20 similar</t>
   </si>
   <si>
     <t>20 repeat</t>
+  </si>
+  <si>
+    <t>20 repeat II</t>
+  </si>
+  <si>
+    <t>40 new</t>
+  </si>
+  <si>
+    <t>40sim</t>
+  </si>
+  <si>
+    <t>40rep</t>
+  </si>
+  <si>
+    <t>60new</t>
+  </si>
+  <si>
+    <t>tot 140</t>
+  </si>
+  <si>
+    <t>Practice/Seagull_A.wav</t>
+  </si>
+  <si>
+    <t>Practice/Gargle_A.wav</t>
+  </si>
+  <si>
+    <t>Practice/Gargle_B.wav</t>
+  </si>
+  <si>
+    <t>Practice/Skid_B.wav</t>
   </si>
 </sst>
 </file>
@@ -944,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7C173C-5764-4F38-AFFA-904419D5AD4C}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -956,7 +980,7 @@
     <col min="2" max="2" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>138</v>
       </c>
@@ -964,402 +988,419 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+      <c r="B10" s="2">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="B11" s="2">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="B12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="B13" s="2">
+        <v>3</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B11" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3</v>
+      </c>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+      <c r="B18" s="2">
+        <v>3</v>
+      </c>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
+      <c r="B19" s="2">
+        <v>3</v>
+      </c>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="B20" s="2">
+        <v>3</v>
+      </c>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
+      <c r="F21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+      <c r="B22" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="2">
-        <v>3</v>
-      </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
+      <c r="B23" s="2">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B19" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
+      <c r="B24" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="20" t="s">
+      <c r="B27" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="18" t="s">
+      <c r="B28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="15" t="s">
+      <c r="B30" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="15" t="s">
         <v>100</v>
-      </c>
-      <c r="B26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B29" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="B30" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="13" t="s">
-        <v>4</v>
       </c>
       <c r="B31" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="19" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B32" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="15" t="s">
+      <c r="B37" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B38" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="18" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B34" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="20" t="s">
+      <c r="B39" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="B35" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+      <c r="B40" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
+      <c r="B41" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
+      <c r="B42" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B39">
+      <c r="B43" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B41" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B43" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44" s="11">
-        <v>3</v>
-      </c>
-    </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
+      <c r="A45" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="11">
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="B46" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="11">
-        <v>3</v>
+      <c r="A47" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
+      <c r="A48" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="11">
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B49" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B50" s="11">
-        <v>3</v>
+      <c r="A50" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="9" t="s">
-        <v>105</v>
+      <c r="A51" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="B51" s="11">
         <v>3</v>
@@ -1367,55 +1408,55 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B52" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="9" t="s">
+      <c r="B57" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="B53" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="B55" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="B56" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B57" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="B58" s="11">
         <v>3</v>
@@ -1423,159 +1464,159 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" s="11">
+        <v>4</v>
+      </c>
+      <c r="B59">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="16" t="s">
-        <v>129</v>
+      <c r="A60" s="20" t="s">
+        <v>134</v>
       </c>
       <c r="B60" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="18" t="s">
-        <v>118</v>
+      <c r="A61" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="B61" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="13" t="s">
-        <v>5</v>
+      <c r="A62" s="15" t="s">
+        <v>77</v>
       </c>
       <c r="B62" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="3" t="s">
-        <v>63</v>
+      <c r="A63" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="B63" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="17" t="s">
-        <v>130</v>
+      <c r="A64" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="B64" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="20" t="s">
-        <v>135</v>
+      <c r="A65" s="16" t="s">
+        <v>129</v>
       </c>
       <c r="B65" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" s="13" t="s">
-        <v>105</v>
+      <c r="A66" s="18" t="s">
+        <v>118</v>
       </c>
       <c r="B66" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="11">
         <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B67" s="11">
-        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="B70" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B72" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B68" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" s="13" t="s">
+      <c r="B73" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="11">
+      <c r="B74" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" s="16" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B70" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" s="18" t="s">
+      <c r="B75" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B71" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" s="3" t="s">
+      <c r="B76" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B72" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" s="15" t="s">
+      <c r="B77" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" s="15" t="s">
         <v>77</v>
-      </c>
-      <c r="B73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B74" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B75" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B77" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" s="13" t="s">
-        <v>5</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -1583,39 +1624,80 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="B79" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B80">
-        <v>1</v>
+      <c r="A80" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B80" s="11">
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="13" t="s">
-        <v>105</v>
+        <v>26</v>
       </c>
       <c r="B81">
         <v>1</v>
       </c>
     </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B82" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B84" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2822FA-E371-492F-BF2E-5CC12045B6A4}">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1625,7 +1707,7 @@
     <col min="8" max="8" width="35.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>138</v>
       </c>
@@ -1636,7 +1718,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
@@ -1649,8 +1731,14 @@
       <c r="J2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
@@ -1661,10 +1749,16 @@
         <v>150</v>
       </c>
       <c r="J3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+      <c r="L3">
+        <v>20</v>
+      </c>
+      <c r="M3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>53</v>
       </c>
@@ -1672,21 +1766,30 @@
         <v>3</v>
       </c>
       <c r="I4" t="s">
+        <v>151</v>
+      </c>
+      <c r="J4" t="s">
         <v>152</v>
       </c>
-      <c r="J4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>81</v>
       </c>
@@ -1694,10 +1797,13 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+      <c r="L6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>32</v>
       </c>
@@ -1706,10 +1812,13 @@
       </c>
       <c r="C7" s="10"/>
       <c r="I7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+      <c r="L7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>105</v>
       </c>
@@ -1717,10 +1826,13 @@
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+      <c r="L8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>26</v>
       </c>
@@ -1728,7 +1840,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>5</v>
       </c>
@@ -1736,7 +1848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
@@ -1747,7 +1859,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>108</v>
       </c>
@@ -1758,7 +1870,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>15</v>
       </c>
@@ -1766,7 +1878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>22</v>
       </c>
@@ -1777,7 +1889,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>26</v>
       </c>
@@ -1788,7 +1900,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>137</v>
       </c>
@@ -2305,10 +2417,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294CB12A-D23A-4261-8EC5-DD7E3139FA57}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2445,7 +2557,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>96</v>
       </c>
@@ -2453,7 +2565,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>72</v>
       </c>
@@ -2461,7 +2573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
@@ -2469,7 +2581,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>104</v>
       </c>
@@ -2477,7 +2589,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>63</v>
       </c>
@@ -2485,7 +2597,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
@@ -2496,7 +2608,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
@@ -2507,7 +2619,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>53</v>
       </c>
@@ -2518,7 +2630,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>11</v>
       </c>
@@ -2528,8 +2640,9 @@
       <c r="D25" s="10" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>81</v>
       </c>
@@ -2539,8 +2652,9 @@
       <c r="D26" s="10" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>86</v>
       </c>
@@ -2550,8 +2664,11 @@
       <c r="D27" s="10" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G27" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
@@ -2561,8 +2678,11 @@
       <c r="D28" s="12" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G28" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>88</v>
       </c>
@@ -2572,8 +2692,11 @@
       <c r="D29" s="12" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G29" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>17</v>
       </c>
@@ -2583,8 +2706,11 @@
       <c r="D30" s="12" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G30" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>90</v>
       </c>
@@ -2595,7 +2721,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>105</v>
       </c>
@@ -2606,7 +2732,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>26</v>
       </c>
@@ -2617,7 +2743,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -2628,7 +2754,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>64</v>
       </c>
@@ -2639,7 +2765,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>42</v>
       </c>
@@ -2650,7 +2776,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>8</v>
       </c>
@@ -2661,7 +2787,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>52</v>
       </c>
@@ -2672,7 +2798,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>25</v>
       </c>
@@ -2683,7 +2809,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>12</v>
       </c>
@@ -2694,7 +2820,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>29</v>
       </c>
@@ -2705,7 +2831,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>54</v>
       </c>
@@ -2715,8 +2841,11 @@
       <c r="D42" s="10" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F42" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>15</v>
       </c>
@@ -2726,8 +2855,11 @@
       <c r="D43" s="10" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F43" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>98</v>
       </c>
@@ -2737,8 +2869,11 @@
       <c r="D44" s="11" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F44" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>35</v>
       </c>
@@ -2748,8 +2883,11 @@
       <c r="D45" s="11" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F45" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>4</v>
       </c>
@@ -2759,8 +2897,11 @@
       <c r="D46" s="8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F46" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>92</v>
       </c>
@@ -2770,8 +2911,11 @@
       <c r="D47" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F47" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>40</v>
       </c>
@@ -2781,8 +2925,11 @@
       <c r="D48" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F48" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>30</v>
       </c>
@@ -2792,8 +2939,11 @@
       <c r="D49" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F49" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>62</v>
       </c>
@@ -2803,8 +2953,11 @@
       <c r="D50" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F50" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>87</v>
       </c>
@@ -2814,175 +2967,238 @@
       <c r="D51" s="8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F51" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>107</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F52" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>108</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F53" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>109</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F54" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F55" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F56" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>111</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F57" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F58" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F59" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F60" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F61" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F62" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F63" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="F64" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="F65" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="F66" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="F67" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="F68" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="F69" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="F70" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="F71" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>136</v>
       </c>
@@ -3103,7 +3319,7 @@
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B82" sqref="B82:B101"/>
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
increased to 110 sounds
</commit_message>
<xml_diff>
--- a/GuessSounds_conditions.xlsx
+++ b/GuessSounds_conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/swan689_uwo_ca/Documents/Desktop/Project BL/Guess The Sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{4AF6C817-0FAB-4552-9560-1836CE493123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{41100F38-E1FD-4556-AE57-21E9DA2CFA91}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{4AF6C817-0FAB-4552-9560-1836CE493123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B402EF26-42C8-4B0D-84D7-DDBC907706FC}"/>
   <bookViews>
-    <workbookView xWindow="10450" yWindow="1020" windowWidth="12110" windowHeight="12810" xr2:uid="{BE90900A-ACE8-4230-85D6-181754847329}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{BE90900A-ACE8-4230-85D6-181754847329}"/>
   </bookViews>
   <sheets>
     <sheet name="V4" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="175">
   <si>
     <t>Type</t>
   </si>
@@ -523,13 +523,43 @@
   </si>
   <si>
     <t>Practice/Skid_B.wav</t>
+  </si>
+  <si>
+    <t>Growl_B.wav</t>
+  </si>
+  <si>
+    <t>Growl_C.wav</t>
+  </si>
+  <si>
+    <t>Coin_B.wav</t>
+  </si>
+  <si>
+    <t>Coin_C.wav</t>
+  </si>
+  <si>
+    <t>Goat_A.wav</t>
+  </si>
+  <si>
+    <t>Goat_C.wav</t>
+  </si>
+  <si>
+    <t>Whistle_B.wav</t>
+  </si>
+  <si>
+    <t>Whistle_C.wav</t>
+  </si>
+  <si>
+    <t>Phone_C.wav</t>
+  </si>
+  <si>
+    <t>Phone_D.wav</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,8 +575,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -619,6 +656,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -632,7 +693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -654,6 +715,18 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7C173C-5764-4F38-AFFA-904419D5AD4C}">
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -980,7 +1053,7 @@
     <col min="2" max="2" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>138</v>
       </c>
@@ -988,7 +1061,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>161</v>
       </c>
@@ -996,7 +1069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>164</v>
       </c>
@@ -1004,7 +1077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>161</v>
       </c>
@@ -1012,7 +1085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>162</v>
       </c>
@@ -1020,7 +1093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>163</v>
       </c>
@@ -1028,16 +1101,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
-        <v>6</v>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B7" s="2">
         <v>3</v>
       </c>
+      <c r="E7" s="11"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>54</v>
       </c>
@@ -1046,7 +1120,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1055,7 +1129,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -1064,7 +1138,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1073,7 +1147,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>81</v>
       </c>
@@ -1081,81 +1155,72 @@
         <v>3</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B13" s="2">
         <v>3</v>
       </c>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="2">
         <v>3</v>
       </c>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B15" s="2">
         <v>3</v>
       </c>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>137</v>
       </c>
       <c r="B16" s="2">
         <v>2</v>
       </c>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>56</v>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B17" s="2">
         <v>3</v>
       </c>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B18" s="2">
         <v>3</v>
       </c>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B19" s="2">
         <v>3</v>
       </c>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="2">
         <v>3</v>
       </c>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
         <v>8</v>
       </c>
@@ -1163,9 +1228,8 @@
         <v>1</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>4</v>
       </c>
@@ -1173,7 +1237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>31</v>
       </c>
@@ -1182,7 +1246,7 @@
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
         <v>124</v>
       </c>
@@ -1190,7 +1254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>92</v>
       </c>
@@ -1198,7 +1262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
         <v>122</v>
       </c>
@@ -1206,15 +1270,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>96</v>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="B27" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="20" t="s">
         <v>115</v>
       </c>
@@ -1222,7 +1286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
         <v>108</v>
       </c>
@@ -1230,7 +1294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>85</v>
       </c>
@@ -1238,7 +1302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
         <v>100</v>
       </c>
@@ -1246,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>66</v>
       </c>
@@ -1254,7 +1318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -1262,7 +1326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
         <v>112</v>
       </c>
@@ -1270,7 +1334,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="16" t="s">
         <v>110</v>
       </c>
@@ -1278,7 +1342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
         <v>4</v>
       </c>
@@ -1286,7 +1350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="19" t="s">
         <v>136</v>
       </c>
@@ -1294,7 +1358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="15" t="s">
         <v>31</v>
       </c>
@@ -1302,7 +1366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
         <v>107</v>
       </c>
@@ -1310,7 +1374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="20" t="s">
         <v>125</v>
       </c>
@@ -1318,7 +1382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>43</v>
       </c>
@@ -1326,7 +1390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>77</v>
       </c>
@@ -1334,23 +1398,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="3" t="s">
-        <v>14</v>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="B43" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44" s="10"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>3</v>
       </c>
@@ -1358,7 +1424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
         <v>17</v>
       </c>
@@ -1366,7 +1432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="15" t="s">
         <v>66</v>
       </c>
@@ -1374,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
         <v>90</v>
       </c>
@@ -1510,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="16" t="s">
         <v>129</v>
       </c>
@@ -1518,7 +1584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="18" t="s">
         <v>118</v>
       </c>
@@ -1526,7 +1592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="13" t="s">
         <v>5</v>
       </c>
@@ -1534,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>1</v>
       </c>
@@ -1542,7 +1608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="17" t="s">
         <v>130</v>
       </c>
@@ -1550,7 +1616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="20" t="s">
         <v>135</v>
       </c>
@@ -1558,7 +1624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="13" t="s">
         <v>105</v>
       </c>
@@ -1566,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="19" t="s">
         <v>120</v>
       </c>
@@ -1574,117 +1640,461 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B73" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" s="3">
+        <v>3</v>
+      </c>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="13" t="s">
         <v>64</v>
       </c>
       <c r="B74" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="16" t="s">
         <v>126</v>
       </c>
       <c r="B75" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C75" s="2"/>
+      <c r="G75" s="3"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="18" t="s">
         <v>119</v>
       </c>
       <c r="B76" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B77" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C76" s="2"/>
+      <c r="G76" s="2"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" s="3">
+        <v>3</v>
+      </c>
+      <c r="C77" s="11"/>
+      <c r="G77" s="2"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="15" t="s">
         <v>77</v>
       </c>
       <c r="B78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C78" s="2"/>
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B79" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C79" s="2"/>
+      <c r="G79" s="2"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B80" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C80" s="2"/>
+      <c r="G80" s="2"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C81" s="2"/>
+      <c r="G81" s="2"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="17" t="s">
         <v>117</v>
       </c>
       <c r="B82" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C82" s="2"/>
+      <c r="G82" s="2"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B84" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C83" s="2"/>
+      <c r="G83" s="2"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B84" s="3">
+        <v>1</v>
+      </c>
+      <c r="C84" s="3"/>
+      <c r="G84" s="2"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="13" t="s">
         <v>64</v>
       </c>
       <c r="B85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C85" s="2"/>
+      <c r="G85" s="2"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="13" t="s">
         <v>105</v>
       </c>
       <c r="B86">
         <v>1</v>
       </c>
+      <c r="C86" s="2"/>
+      <c r="G86" s="2"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B87" s="2">
+        <v>3</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="G87" s="3"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="B88" s="2">
+        <v>2</v>
+      </c>
+      <c r="C88" s="32"/>
+      <c r="G88" s="2"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B89" s="3">
+        <v>3</v>
+      </c>
+      <c r="C89" s="2"/>
+      <c r="G89" s="2"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B90" s="3">
+        <v>3</v>
+      </c>
+      <c r="C90" s="2"/>
+      <c r="G90" s="2"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B91" s="2">
+        <v>3</v>
+      </c>
+      <c r="C91" s="3"/>
+      <c r="D91" s="2"/>
+      <c r="G91" s="2"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B92" s="2">
+        <v>3</v>
+      </c>
+      <c r="C92" s="2"/>
+      <c r="D92" s="3"/>
+      <c r="G92" s="2"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" s="2">
+        <v>1</v>
+      </c>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="G93" s="2"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B94" s="2">
+        <v>3</v>
+      </c>
+      <c r="C94" s="3"/>
+      <c r="D94" s="2"/>
+      <c r="G94" s="2"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B95" s="2">
+        <v>3</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="G95" s="2"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A96" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="B96" s="2">
+        <v>2</v>
+      </c>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="G96" s="2"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A97" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B97" s="2">
+        <v>2</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" s="3"/>
+      <c r="G97" s="2"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A98" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B98" s="2">
+        <v>3</v>
+      </c>
+      <c r="C98" s="2"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="2"/>
+      <c r="G98" s="2"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B99" s="2">
+        <v>3</v>
+      </c>
+      <c r="C99" s="2"/>
+      <c r="D99" s="3"/>
+      <c r="G99" s="2"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A100" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B100" s="2">
+        <v>1</v>
+      </c>
+      <c r="C100" s="2"/>
+      <c r="D100" s="3"/>
+      <c r="G100" s="2"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A101" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="B101" s="2">
+        <v>2</v>
+      </c>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="G101" s="2"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B102" s="2">
+        <v>3</v>
+      </c>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="G102" s="3"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A103" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B103" s="2">
+        <v>2</v>
+      </c>
+      <c r="C103" s="2"/>
+      <c r="D103" s="3"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A104" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B104" s="11">
+        <v>1</v>
+      </c>
+      <c r="C104" s="2"/>
+      <c r="D104" s="3"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A105" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B105" s="11">
+        <v>1</v>
+      </c>
+      <c r="C105" s="11"/>
+      <c r="D105" s="3"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A106" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="B106" s="2">
+        <v>2</v>
+      </c>
+      <c r="C106" s="2"/>
+      <c r="D106" s="3"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A107" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B107" s="11">
+        <v>1</v>
+      </c>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A108" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108" s="2">
+        <v>2</v>
+      </c>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A109" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B109" s="2">
+        <v>2</v>
+      </c>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A110" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="B110" s="2">
+        <v>2</v>
+      </c>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A111" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B111" s="2">
+        <v>1</v>
+      </c>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A112" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B112" s="2">
+        <v>1</v>
+      </c>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A113" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B113" s="2">
+        <v>1</v>
+      </c>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A114" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="B114" s="2">
+        <v>2</v>
+      </c>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A115" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B115" s="2">
+        <v>1</v>
+      </c>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B117" s="11"/>
+      <c r="C117" s="11"/>
+      <c r="D117" s="2"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D118" s="2"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C119" s="11"/>
+      <c r="D119" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed two sound files
</commit_message>
<xml_diff>
--- a/GuessSounds_conditions.xlsx
+++ b/GuessSounds_conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/swan689_uwo_ca/Documents/Desktop/Project BL/Guess The Sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="8_{4AF6C817-0FAB-4552-9560-1836CE493123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8A769032-CE5A-466F-9439-82D1164BE2CA}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="8_{4AF6C817-0FAB-4552-9560-1836CE493123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{23628650-0A11-4AA5-BF68-3986635C6BA3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{BE90900A-ACE8-4230-85D6-181754847329}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2491" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2491" uniqueCount="200">
   <si>
     <t>Type</t>
   </si>
@@ -626,6 +626,12 @@
   </si>
   <si>
     <t>Faucet_B.wav</t>
+  </si>
+  <si>
+    <t>Snore_C.wav</t>
+  </si>
+  <si>
+    <t>Writing_C.wav</t>
   </si>
 </sst>
 </file>
@@ -1154,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B591AA4-9955-44B8-BDCB-F372396C550D}">
   <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1571,7 +1577,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="46" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -2089,7 +2095,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="46" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B67">
         <v>2</v>

</xml_diff>

<commit_message>
Added 5 "high" similar sounds
</commit_message>
<xml_diff>
--- a/GuessSounds_conditions.xlsx
+++ b/GuessSounds_conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/swan689_uwo_ca/Documents/Desktop/Project BL/Guess The Sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="8_{4AF6C817-0FAB-4552-9560-1836CE493123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AD1DBA5A-CF09-40D5-A2F1-7585208CE529}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="8_{4AF6C817-0FAB-4552-9560-1836CE493123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AB931682-AA12-422F-A46B-6254B0C0664F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{BE90900A-ACE8-4230-85D6-181754847329}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="152">
   <si>
     <t>Type</t>
   </si>
@@ -477,6 +477,15 @@
   </si>
   <si>
     <t>Test/Lures/Bubbles_B.wav</t>
+  </si>
+  <si>
+    <t>Clap_B.wav</t>
+  </si>
+  <si>
+    <t>Clap_C.wav</t>
+  </si>
+  <si>
+    <t>CarStart_E.wav</t>
   </si>
 </sst>
 </file>
@@ -647,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -698,6 +707,7 @@
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B591AA4-9955-44B8-BDCB-F372396C550D}">
   <dimension ref="A1:J134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G80" sqref="G80"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="G126" sqref="G126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1210,44 +1220,44 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="11">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="11">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="11">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" s="11">
-        <v>3</v>
-      </c>
-      <c r="D15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
-        <v>14</v>
-      </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -1267,92 +1277,92 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" s="11">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="11">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" s="11">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="11">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" s="11">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20" s="11">
-        <v>3</v>
-      </c>
-      <c r="D20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="46" t="s">
-        <v>63</v>
-      </c>
       <c r="B22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="21" t="s">
-        <v>19</v>
+      <c r="A23" s="44" t="s">
+        <v>16</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="44" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1367,35 +1377,35 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="44" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="44" t="s">
-        <v>41</v>
+      <c r="A26" s="39" t="s">
+        <v>66</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
       <c r="C26" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="39" t="s">
-        <v>66</v>
+      <c r="A27" s="21" t="s">
+        <v>3</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -2319,7 +2329,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="44" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -2430,8 +2440,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A101" s="28" t="s">
-        <v>5</v>
+      <c r="A101" s="50" t="s">
+        <v>137</v>
       </c>
       <c r="B101">
         <v>2</v>
@@ -2543,7 +2553,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="44" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -2612,8 +2622,8 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A114" s="39" t="s">
-        <v>8</v>
+      <c r="A114" s="47" t="s">
+        <v>149</v>
       </c>
       <c r="B114">
         <v>2</v>
@@ -2640,7 +2650,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A116" s="28" t="s">
+      <c r="A116" s="50" t="s">
         <v>136</v>
       </c>
       <c r="B116">
@@ -2696,7 +2706,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A120" s="39" t="s">
+      <c r="A120" s="47" t="s">
         <v>88</v>
       </c>
       <c r="B120">
@@ -2864,8 +2874,8 @@
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A132" s="21" t="s">
-        <v>53</v>
+      <c r="A132" s="48" t="s">
+        <v>151</v>
       </c>
       <c r="B132">
         <v>2</v>
@@ -2892,8 +2902,8 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A134" s="39" t="s">
-        <v>96</v>
+      <c r="A134" s="47" t="s">
+        <v>150</v>
       </c>
       <c r="B134">
         <v>2</v>

</xml_diff>

<commit_message>
Changed a few sound files
</commit_message>
<xml_diff>
--- a/GuessSounds_conditions.xlsx
+++ b/GuessSounds_conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/swan689_uwo_ca/Documents/Desktop/Project BL/Guess The Sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="8_{4AF6C817-0FAB-4552-9560-1836CE493123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AB931682-AA12-422F-A46B-6254B0C0664F}"/>
+  <xr:revisionPtr revIDLastSave="273" documentId="8_{4AF6C817-0FAB-4552-9560-1836CE493123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1A248390-979B-4D15-A37E-B5E80EF54E9E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{BE90900A-ACE8-4230-85D6-181754847329}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="165">
   <si>
     <t>Type</t>
   </si>
@@ -464,9 +464,6 @@
     <t>Writing_C.wav</t>
   </si>
   <si>
-    <t>Elephant_B.wav</t>
-  </si>
-  <si>
     <t>Cough_E.wav</t>
   </si>
   <si>
@@ -486,6 +483,48 @@
   </si>
   <si>
     <t>CarStart_E.wav</t>
+  </si>
+  <si>
+    <t>Baby_E.wav</t>
+  </si>
+  <si>
+    <t>Baby_F.wav</t>
+  </si>
+  <si>
+    <t>Dog_F.wav</t>
+  </si>
+  <si>
+    <t>Dog_E.wav</t>
+  </si>
+  <si>
+    <t>Elephant_C.wav</t>
+  </si>
+  <si>
+    <t>Elephant_D.wav</t>
+  </si>
+  <si>
+    <t>Snore_D.wav</t>
+  </si>
+  <si>
+    <t>Chomp_E.wav</t>
+  </si>
+  <si>
+    <t>Growl_F.wav</t>
+  </si>
+  <si>
+    <t>Growl_E.wav</t>
+  </si>
+  <si>
+    <t>Duck_A.wav</t>
+  </si>
+  <si>
+    <t>Goat_D.wav</t>
+  </si>
+  <si>
+    <t>Coin_E.wav</t>
+  </si>
+  <si>
+    <t>Coin_D.wav</t>
   </si>
 </sst>
 </file>
@@ -1024,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B591AA4-9955-44B8-BDCB-F372396C550D}">
   <dimension ref="A1:J134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="G126" sqref="G126"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1037,7 +1076,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>98</v>
@@ -1121,7 +1160,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="28" t="s">
-        <v>18</v>
+        <v>155</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1233,8 +1272,8 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="21" t="s">
-        <v>14</v>
+      <c r="A15" s="48" t="s">
+        <v>152</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1291,7 +1330,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1316,6 +1355,7 @@
       <c r="D20" t="s">
         <v>127</v>
       </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
@@ -1348,7 +1388,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="44" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1362,31 +1402,31 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="44" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="44" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -1432,8 +1472,8 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="39" t="s">
-        <v>83</v>
+      <c r="A29" s="46" t="s">
+        <v>143</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -1446,59 +1486,59 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="46" t="s">
-        <v>143</v>
+      <c r="A30" s="28" t="s">
+        <v>24</v>
       </c>
       <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="C30" s="11">
-        <v>2</v>
-      </c>
-      <c r="D30" t="s">
-        <v>128</v>
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" s="28" t="s">
-        <v>24</v>
+      <c r="A31" s="21" t="s">
+        <v>56</v>
       </c>
       <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>129</v>
+        <v>2</v>
+      </c>
+      <c r="C31" s="11">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="21" t="s">
-        <v>56</v>
+      <c r="A32" s="44" t="s">
+        <v>58</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="44" t="s">
-        <v>58</v>
+      <c r="A33" s="28" t="s">
+        <v>25</v>
       </c>
       <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" s="11">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>129</v>
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -1544,17 +1584,17 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="28" t="s">
-        <v>25</v>
+      <c r="A37" s="47" t="s">
+        <v>151</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>127</v>
+      <c r="C37" s="11">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
@@ -1572,8 +1612,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="28" t="s">
-        <v>64</v>
+      <c r="A39" s="50" t="s">
+        <v>161</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -1685,7 +1725,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -1711,65 +1751,65 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="47" t="s">
-        <v>147</v>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="44" t="s">
+        <v>60</v>
       </c>
       <c r="B49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C49" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="44" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="44" t="s">
-        <v>38</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="28" t="s">
+        <v>25</v>
       </c>
       <c r="B51">
-        <v>2</v>
-      </c>
-      <c r="C51" s="11">
-        <v>3</v>
-      </c>
-      <c r="D51" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="28" t="s">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="47" t="s">
+        <v>146</v>
       </c>
       <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="21" t="s">
-        <v>140</v>
+        <v>2</v>
+      </c>
+      <c r="C52" s="11">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="48" t="s">
+        <v>157</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -1781,7 +1821,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="44" t="s">
         <v>123</v>
       </c>
@@ -1795,7 +1835,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="44" t="s">
         <v>54</v>
       </c>
@@ -1809,8 +1849,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="21" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="48" t="s">
         <v>40</v>
       </c>
       <c r="B56">
@@ -1822,9 +1862,10 @@
       <c r="D56" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="28" t="s">
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="50" t="s">
         <v>139</v>
       </c>
       <c r="B57">
@@ -1836,8 +1877,9 @@
       <c r="D57" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="39" t="s">
         <v>94</v>
       </c>
@@ -1851,7 +1893,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="44" t="s">
         <v>2</v>
       </c>
@@ -1865,7 +1907,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="28" t="s">
         <v>31</v>
       </c>
@@ -1879,7 +1921,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="28" t="s">
         <v>62</v>
       </c>
@@ -1893,8 +1935,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="39" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B62">
@@ -1907,7 +1949,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="44" t="s">
         <v>29</v>
       </c>
@@ -1921,7 +1963,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="48" t="s">
         <v>35</v>
       </c>
@@ -1935,7 +1977,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="28" t="s">
         <v>39</v>
       </c>
@@ -1949,7 +1991,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="44" t="s">
         <v>32</v>
       </c>
@@ -1963,8 +2005,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="46" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" s="50" t="s">
         <v>142</v>
       </c>
       <c r="B67">
@@ -1977,7 +2019,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="28" t="s">
         <v>51</v>
       </c>
@@ -1991,8 +2033,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69" s="39" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" s="47" t="s">
         <v>115</v>
       </c>
       <c r="B69">
@@ -2005,49 +2047,49 @@
         <v>128</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" s="44" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70" s="11">
+        <v>3</v>
+      </c>
+      <c r="D70" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="B70">
-        <v>1</v>
-      </c>
-      <c r="C70" s="11">
-        <v>1</v>
-      </c>
-      <c r="D70" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" s="44" t="s">
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71" s="11">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="B71">
-        <v>1</v>
-      </c>
-      <c r="C71" s="11">
-        <v>1</v>
-      </c>
-      <c r="D71" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72" s="39" t="s">
-        <v>117</v>
-      </c>
       <c r="B72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C72" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D72" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="44" t="s">
         <v>30</v>
       </c>
@@ -2061,107 +2103,108 @@
         <v>127</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A74" s="39" t="s">
-        <v>78</v>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" s="28" t="s">
+        <v>62</v>
       </c>
       <c r="B74">
-        <v>2</v>
-      </c>
-      <c r="C74" s="11">
-        <v>2</v>
-      </c>
-      <c r="D74" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="28" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" s="28" t="s">
-        <v>49</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" s="44" t="s">
+        <v>15</v>
       </c>
       <c r="B76">
         <v>2</v>
       </c>
-      <c r="C76">
-        <v>3</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" s="48" t="s">
+      <c r="C76" s="11">
+        <v>3</v>
+      </c>
+      <c r="D76" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77">
+        <v>2</v>
+      </c>
+      <c r="C77" s="11">
+        <v>3</v>
+      </c>
+      <c r="D77" t="s">
+        <v>127</v>
+      </c>
+      <c r="E77" s="2"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B77">
-        <v>1</v>
-      </c>
-      <c r="C77" s="11">
-        <v>1</v>
-      </c>
-      <c r="D77" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78" s="44" t="s">
-        <v>15</v>
-      </c>
       <c r="B78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C78" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79" s="21" t="s">
-        <v>10</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" s="50" t="s">
+        <v>57</v>
       </c>
       <c r="B79">
         <v>2</v>
       </c>
-      <c r="C79" s="11">
-        <v>3</v>
-      </c>
-      <c r="D79" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A80" s="28" t="s">
-        <v>57</v>
+      <c r="C79">
+        <v>3</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" s="47" t="s">
+        <v>158</v>
       </c>
       <c r="B80">
         <v>2</v>
       </c>
-      <c r="C80">
-        <v>3</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>127</v>
+      <c r="C80" s="11">
+        <v>2</v>
+      </c>
+      <c r="D80" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="44" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -2175,44 +2218,44 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="44" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C82" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D82" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A83" s="44" t="s">
-        <v>48</v>
+      <c r="A83" s="21" t="s">
+        <v>36</v>
       </c>
       <c r="B83">
         <v>2</v>
       </c>
       <c r="C83" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A84" s="21" t="s">
-        <v>36</v>
+      <c r="A84" s="44" t="s">
+        <v>30</v>
       </c>
       <c r="B84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C84" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
@@ -2244,45 +2287,45 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A87" s="44" t="s">
-        <v>6</v>
+      <c r="A87" s="28" t="s">
+        <v>23</v>
       </c>
       <c r="B87">
         <v>2</v>
       </c>
-      <c r="C87" s="11">
-        <v>3</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88">
+        <v>2</v>
+      </c>
+      <c r="C88" s="11">
+        <v>3</v>
+      </c>
+      <c r="D88" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B88">
-        <v>1</v>
-      </c>
-      <c r="C88" s="11">
-        <v>1</v>
-      </c>
-      <c r="D88" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A89" s="28" t="s">
-        <v>23</v>
-      </c>
       <c r="B89">
-        <v>2</v>
-      </c>
-      <c r="C89">
-        <v>3</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>127</v>
+        <v>1</v>
+      </c>
+      <c r="C89" s="11">
+        <v>1</v>
+      </c>
+      <c r="D89" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
@@ -2300,8 +2343,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A91" s="21" t="s">
-        <v>7</v>
+      <c r="A91" s="48" t="s">
+        <v>154</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -2371,7 +2414,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="39" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B96">
         <v>2</v>
@@ -2384,7 +2427,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A97" s="28" t="s">
+      <c r="A97" s="50" t="s">
         <v>133</v>
       </c>
       <c r="B97">
@@ -2398,8 +2441,8 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A98" s="39" t="s">
-        <v>22</v>
+      <c r="A98" s="47" t="s">
+        <v>162</v>
       </c>
       <c r="B98">
         <v>2</v>
@@ -2441,7 +2484,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="50" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="B101">
         <v>2</v>
@@ -2524,8 +2567,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A107" s="21" t="s">
-        <v>11</v>
+      <c r="A107" s="48" t="s">
+        <v>160</v>
       </c>
       <c r="B107">
         <v>2</v>
@@ -2566,8 +2609,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A110" s="39" t="s">
-        <v>89</v>
+      <c r="A110" s="47" t="s">
+        <v>153</v>
       </c>
       <c r="B110">
         <v>2</v>
@@ -2623,7 +2666,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B114">
         <v>2</v>
@@ -2651,7 +2694,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" s="50" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="B116">
         <v>2</v>
@@ -2707,7 +2750,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" s="47" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="B120">
         <v>2</v>
@@ -2734,8 +2777,8 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A122" s="39" t="s">
-        <v>111</v>
+      <c r="A122" s="47" t="s">
+        <v>159</v>
       </c>
       <c r="B122">
         <v>2</v>
@@ -2748,7 +2791,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A123" s="39" t="s">
+      <c r="A123" s="47" t="s">
         <v>113</v>
       </c>
       <c r="B123">
@@ -2791,7 +2834,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" s="49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B126">
         <v>2</v>
@@ -2875,7 +2918,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" s="48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B132">
         <v>2</v>
@@ -2903,7 +2946,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" s="47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B134">
         <v>2</v>
@@ -2937,7 +2980,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>130</v>
@@ -4720,7 +4763,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>98</v>
@@ -6841,7 +6884,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
Changed audio file for Dog
</commit_message>
<xml_diff>
--- a/GuessSounds_conditions.xlsx
+++ b/GuessSounds_conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/swan689_uwo_ca/Documents/Desktop/Project BL/Guess The Sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="339" documentId="8_{4AF6C817-0FAB-4552-9560-1836CE493123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8308CF6C-7FE1-4C66-9B0C-8BF3CF9956CB}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="8_{4AF6C817-0FAB-4552-9560-1836CE493123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{79B78143-30BE-4EA2-B5BF-61C2D6AA1E6F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{BE90900A-ACE8-4230-85D6-181754847329}"/>
   </bookViews>
@@ -581,9 +581,6 @@
     <t>Goat_E.wav</t>
   </si>
   <si>
-    <t>Dog_H.wav</t>
-  </si>
-  <si>
     <t>Cough_G.wav</t>
   </si>
   <si>
@@ -593,10 +590,13 @@
     <t>Duck_C.wav</t>
   </si>
   <si>
-    <t>Dog_G.wav</t>
-  </si>
-  <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Dog_E.wav</t>
+  </si>
+  <si>
+    <t>Dog_F.wav</t>
   </si>
 </sst>
 </file>
@@ -1136,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B591AA4-9955-44B8-BDCB-F372396C550D}">
   <dimension ref="A1:E390"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H272" sqref="H272"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="H106" sqref="H106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -3002,7 +3002,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="47" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B110">
         <v>2</v>
@@ -3665,7 +3665,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B149">
         <v>2</v>
@@ -3988,7 +3988,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B168">
         <v>2</v>
@@ -4311,7 +4311,7 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="47" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B187">
         <v>2</v>
@@ -5348,7 +5348,7 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B248">
         <v>2</v>
@@ -5615,7 +5615,7 @@
         <v>127</v>
       </c>
       <c r="E263" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.35">
@@ -5632,7 +5632,7 @@
         <v>127</v>
       </c>
       <c r="E264" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.35">
@@ -5649,7 +5649,7 @@
         <v>127</v>
       </c>
       <c r="E265" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.35">
@@ -5666,7 +5666,7 @@
         <v>127</v>
       </c>
       <c r="E266" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.35">
@@ -5683,7 +5683,7 @@
         <v>127</v>
       </c>
       <c r="E267" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.35">
@@ -5700,7 +5700,7 @@
         <v>127</v>
       </c>
       <c r="E268" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.35">
@@ -5717,7 +5717,7 @@
         <v>127</v>
       </c>
       <c r="E269" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.35">
@@ -5734,7 +5734,7 @@
         <v>127</v>
       </c>
       <c r="E270" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.35">
@@ -5751,7 +5751,7 @@
         <v>127</v>
       </c>
       <c r="E271" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.35">
@@ -5768,7 +5768,7 @@
         <v>128</v>
       </c>
       <c r="E272" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.35">
@@ -5785,7 +5785,7 @@
         <v>127</v>
       </c>
       <c r="E273" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.35">
@@ -5802,7 +5802,7 @@
         <v>127</v>
       </c>
       <c r="E274" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.35">
@@ -5819,7 +5819,7 @@
         <v>127</v>
       </c>
       <c r="E275" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.35">
@@ -5836,7 +5836,7 @@
         <v>127</v>
       </c>
       <c r="E276" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.35">
@@ -5853,7 +5853,7 @@
         <v>127</v>
       </c>
       <c r="E277" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.35">
@@ -5870,7 +5870,7 @@
         <v>129</v>
       </c>
       <c r="E278" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.35">
@@ -5887,7 +5887,7 @@
         <v>127</v>
       </c>
       <c r="E279" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.35">
@@ -5904,7 +5904,7 @@
         <v>128</v>
       </c>
       <c r="E280" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.35">
@@ -5921,24 +5921,24 @@
         <v>127</v>
       </c>
       <c r="E281" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
+        <v>185</v>
+      </c>
+      <c r="B282">
+        <v>2</v>
+      </c>
+      <c r="C282">
+        <v>3</v>
+      </c>
+      <c r="D282" t="s">
+        <v>127</v>
+      </c>
+      <c r="E282" t="s">
         <v>186</v>
-      </c>
-      <c r="B282">
-        <v>2</v>
-      </c>
-      <c r="C282">
-        <v>3</v>
-      </c>
-      <c r="D282" t="s">
-        <v>127</v>
-      </c>
-      <c r="E282" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.35">
@@ -5955,7 +5955,7 @@
         <v>127</v>
       </c>
       <c r="E283" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.35">
@@ -5972,7 +5972,7 @@
         <v>127</v>
       </c>
       <c r="E284" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.35">
@@ -5989,7 +5989,7 @@
         <v>129</v>
       </c>
       <c r="E285" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.35">
@@ -6006,7 +6006,7 @@
         <v>129</v>
       </c>
       <c r="E286" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.35">
@@ -6023,7 +6023,7 @@
         <v>127</v>
       </c>
       <c r="E287" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.35">
@@ -6040,7 +6040,7 @@
         <v>128</v>
       </c>
       <c r="E288" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.35">
@@ -6057,7 +6057,7 @@
         <v>127</v>
       </c>
       <c r="E289" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.35">
@@ -6074,7 +6074,7 @@
         <v>127</v>
       </c>
       <c r="E290" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.35">
@@ -6091,7 +6091,7 @@
         <v>127</v>
       </c>
       <c r="E291" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.35">
@@ -6108,7 +6108,7 @@
         <v>128</v>
       </c>
       <c r="E292" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.35">
@@ -6125,7 +6125,7 @@
         <v>127</v>
       </c>
       <c r="E293" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.35">
@@ -6142,7 +6142,7 @@
         <v>129</v>
       </c>
       <c r="E294" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.35">
@@ -6159,7 +6159,7 @@
         <v>129</v>
       </c>
       <c r="E295" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.35">
@@ -6176,7 +6176,7 @@
         <v>129</v>
       </c>
       <c r="E296" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.35">
@@ -6193,7 +6193,7 @@
         <v>127</v>
       </c>
       <c r="E297" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.35">
@@ -6210,7 +6210,7 @@
         <v>129</v>
       </c>
       <c r="E298" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.35">
@@ -6227,7 +6227,7 @@
         <v>128</v>
       </c>
       <c r="E299" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.35">
@@ -6244,7 +6244,7 @@
         <v>129</v>
       </c>
       <c r="E300" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.35">
@@ -6261,7 +6261,7 @@
         <v>127</v>
       </c>
       <c r="E301" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.35">
@@ -6278,7 +6278,7 @@
         <v>129</v>
       </c>
       <c r="E302" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.35">
@@ -6295,7 +6295,7 @@
         <v>127</v>
       </c>
       <c r="E303" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.35">
@@ -6312,7 +6312,7 @@
         <v>128</v>
       </c>
       <c r="E304" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.35">
@@ -6329,7 +6329,7 @@
         <v>127</v>
       </c>
       <c r="E305" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.35">
@@ -6346,7 +6346,7 @@
         <v>128</v>
       </c>
       <c r="E306" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.35">
@@ -6363,7 +6363,7 @@
         <v>129</v>
       </c>
       <c r="E307" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.35">
@@ -6380,7 +6380,7 @@
         <v>127</v>
       </c>
       <c r="E308" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.35">
@@ -6397,7 +6397,7 @@
         <v>129</v>
       </c>
       <c r="E309" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.35">
@@ -6414,7 +6414,7 @@
         <v>128</v>
       </c>
       <c r="E310" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.35">
@@ -6431,7 +6431,7 @@
         <v>127</v>
       </c>
       <c r="E311" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.35">
@@ -6448,7 +6448,7 @@
         <v>129</v>
       </c>
       <c r="E312" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.35">
@@ -6465,7 +6465,7 @@
         <v>127</v>
       </c>
       <c r="E313" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.35">
@@ -6482,7 +6482,7 @@
         <v>128</v>
       </c>
       <c r="E314" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.35">
@@ -6499,7 +6499,7 @@
         <v>127</v>
       </c>
       <c r="E315" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.35">
@@ -6516,7 +6516,7 @@
         <v>129</v>
       </c>
       <c r="E316" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.35">
@@ -6533,7 +6533,7 @@
         <v>127</v>
       </c>
       <c r="E317" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.35">
@@ -6550,7 +6550,7 @@
         <v>129</v>
       </c>
       <c r="E318" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.35">
@@ -6567,7 +6567,7 @@
         <v>128</v>
       </c>
       <c r="E319" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.35">
@@ -6584,7 +6584,7 @@
         <v>127</v>
       </c>
       <c r="E320" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.35">
@@ -6601,7 +6601,7 @@
         <v>128</v>
       </c>
       <c r="E321" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.35">
@@ -6618,7 +6618,7 @@
         <v>127</v>
       </c>
       <c r="E322" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.35">
@@ -6635,7 +6635,7 @@
         <v>127</v>
       </c>
       <c r="E323" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.35">
@@ -6652,7 +6652,7 @@
         <v>129</v>
       </c>
       <c r="E324" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.35">
@@ -6669,7 +6669,7 @@
         <v>129</v>
       </c>
       <c r="E325" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.35">
@@ -6686,7 +6686,7 @@
         <v>127</v>
       </c>
       <c r="E326" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.35">
@@ -6703,7 +6703,7 @@
         <v>129</v>
       </c>
       <c r="E327" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.35">
@@ -6720,7 +6720,7 @@
         <v>127</v>
       </c>
       <c r="E328" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.35">
@@ -6737,7 +6737,7 @@
         <v>127</v>
       </c>
       <c r="E329" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.35">
@@ -6754,7 +6754,7 @@
         <v>129</v>
       </c>
       <c r="E330" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.35">
@@ -6771,12 +6771,12 @@
         <v>127</v>
       </c>
       <c r="E331" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="47" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B332">
         <v>2</v>
@@ -6788,7 +6788,7 @@
         <v>128</v>
       </c>
       <c r="E332" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.35">
@@ -6805,7 +6805,7 @@
         <v>129</v>
       </c>
       <c r="E333" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.35">
@@ -6822,7 +6822,7 @@
         <v>127</v>
       </c>
       <c r="E334" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.35">
@@ -6839,7 +6839,7 @@
         <v>127</v>
       </c>
       <c r="E335" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.35">
@@ -6856,7 +6856,7 @@
         <v>127</v>
       </c>
       <c r="E336" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.35">
@@ -6873,7 +6873,7 @@
         <v>128</v>
       </c>
       <c r="E337" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.35">
@@ -6890,7 +6890,7 @@
         <v>129</v>
       </c>
       <c r="E338" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.35">
@@ -6907,7 +6907,7 @@
         <v>127</v>
       </c>
       <c r="E339" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.35">
@@ -6924,7 +6924,7 @@
         <v>129</v>
       </c>
       <c r="E340" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.35">
@@ -6941,7 +6941,7 @@
         <v>127</v>
       </c>
       <c r="E341" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.35">
@@ -6958,7 +6958,7 @@
         <v>129</v>
       </c>
       <c r="E342" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.35">
@@ -6975,7 +6975,7 @@
         <v>127</v>
       </c>
       <c r="E343" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.35">
@@ -6992,7 +6992,7 @@
         <v>127</v>
       </c>
       <c r="E344" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.35">
@@ -7009,7 +7009,7 @@
         <v>128</v>
       </c>
       <c r="E345" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.35">
@@ -7026,7 +7026,7 @@
         <v>127</v>
       </c>
       <c r="E346" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.35">
@@ -7043,7 +7043,7 @@
         <v>128</v>
       </c>
       <c r="E347" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.35">
@@ -7060,7 +7060,7 @@
         <v>127</v>
       </c>
       <c r="E348" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.35">
@@ -7077,7 +7077,7 @@
         <v>128</v>
       </c>
       <c r="E349" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.35">
@@ -7094,7 +7094,7 @@
         <v>127</v>
       </c>
       <c r="E350" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.35">
@@ -7111,7 +7111,7 @@
         <v>128</v>
       </c>
       <c r="E351" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.35">
@@ -7128,7 +7128,7 @@
         <v>129</v>
       </c>
       <c r="E352" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.35">
@@ -7145,7 +7145,7 @@
         <v>127</v>
       </c>
       <c r="E353" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.35">
@@ -7162,7 +7162,7 @@
         <v>129</v>
       </c>
       <c r="E354" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.35">
@@ -7179,7 +7179,7 @@
         <v>127</v>
       </c>
       <c r="E355" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.35">
@@ -7196,7 +7196,7 @@
         <v>128</v>
       </c>
       <c r="E356" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.35">
@@ -7213,7 +7213,7 @@
         <v>127</v>
       </c>
       <c r="E357" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.35">
@@ -7230,7 +7230,7 @@
         <v>129</v>
       </c>
       <c r="E358" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.35">
@@ -7247,7 +7247,7 @@
         <v>127</v>
       </c>
       <c r="E359" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.35">
@@ -7264,7 +7264,7 @@
         <v>129</v>
       </c>
       <c r="E360" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.35">
@@ -7281,12 +7281,12 @@
         <v>129</v>
       </c>
       <c r="E361" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B362">
         <v>2</v>
@@ -7298,7 +7298,7 @@
         <v>127</v>
       </c>
       <c r="E362" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.35">
@@ -7315,7 +7315,7 @@
         <v>127</v>
       </c>
       <c r="E363" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.35">
@@ -7332,7 +7332,7 @@
         <v>128</v>
       </c>
       <c r="E364" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.35">
@@ -7349,7 +7349,7 @@
         <v>128</v>
       </c>
       <c r="E365" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.35">
@@ -7366,7 +7366,7 @@
         <v>127</v>
       </c>
       <c r="E366" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.35">
@@ -7383,7 +7383,7 @@
         <v>129</v>
       </c>
       <c r="E367" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.35">
@@ -7400,7 +7400,7 @@
         <v>127</v>
       </c>
       <c r="E368" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.35">
@@ -7417,7 +7417,7 @@
         <v>129</v>
       </c>
       <c r="E369" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.35">
@@ -7434,7 +7434,7 @@
         <v>127</v>
       </c>
       <c r="E370" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.35">
@@ -7451,7 +7451,7 @@
         <v>129</v>
       </c>
       <c r="E371" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.35">
@@ -7468,7 +7468,7 @@
         <v>127</v>
       </c>
       <c r="E372" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.35">
@@ -7485,7 +7485,7 @@
         <v>128</v>
       </c>
       <c r="E373" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.35">
@@ -7502,7 +7502,7 @@
         <v>127</v>
       </c>
       <c r="E374" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.35">
@@ -7519,7 +7519,7 @@
         <v>129</v>
       </c>
       <c r="E375" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.35">
@@ -7536,7 +7536,7 @@
         <v>127</v>
       </c>
       <c r="E376" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.35">
@@ -7553,7 +7553,7 @@
         <v>129</v>
       </c>
       <c r="E377" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.35">
@@ -7570,7 +7570,7 @@
         <v>127</v>
       </c>
       <c r="E378" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.35">
@@ -7587,7 +7587,7 @@
         <v>129</v>
       </c>
       <c r="E379" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.35">
@@ -7604,7 +7604,7 @@
         <v>127</v>
       </c>
       <c r="E380" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.35">
@@ -7621,7 +7621,7 @@
         <v>128</v>
       </c>
       <c r="E381" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.35">
@@ -7638,12 +7638,12 @@
         <v>129</v>
       </c>
       <c r="E382" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A383" s="39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B383">
         <v>2</v>
@@ -7655,7 +7655,7 @@
         <v>128</v>
       </c>
       <c r="E383" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.35">
@@ -7672,7 +7672,7 @@
         <v>129</v>
       </c>
       <c r="E384" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.35">
@@ -7689,7 +7689,7 @@
         <v>129</v>
       </c>
       <c r="E385" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.35">
@@ -7706,7 +7706,7 @@
         <v>129</v>
       </c>
       <c r="E386" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.35">
@@ -7723,7 +7723,7 @@
         <v>129</v>
       </c>
       <c r="E387" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.35">
@@ -7740,7 +7740,7 @@
         <v>128</v>
       </c>
       <c r="E388" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.35">
@@ -7757,7 +7757,7 @@
         <v>129</v>
       </c>
       <c r="E389" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.35">
@@ -7774,7 +7774,7 @@
         <v>129</v>
       </c>
       <c r="E390" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>